<commit_message>
Fixed data - LDA
</commit_message>
<xml_diff>
--- a/data/mixture/8 solutions/LDA_without_112_121.xlsx
+++ b/data/mixture/8 solutions/LDA_without_112_121.xlsx
@@ -452,10 +452,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-3.567702745183611</v>
+        <v>3.567702745183609</v>
       </c>
       <c r="B2" t="n">
-        <v>1.872286650358319</v>
+        <v>1.87228665035832</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -465,10 +465,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-3.893028010530688</v>
+        <v>3.893028010530687</v>
       </c>
       <c r="B3" t="n">
-        <v>1.174235147431014</v>
+        <v>1.174235147431016</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -478,10 +478,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-3.044961475807762</v>
+        <v>3.044961475807763</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.028632240290881</v>
+        <v>-1.02863224029088</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -491,10 +491,10 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-3.034250959510602</v>
+        <v>3.034250959510603</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.358814581522337</v>
+        <v>-1.358814581522336</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -504,10 +504,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-3.069544413844199</v>
+        <v>3.0695444138442</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.36859982538818</v>
+        <v>-1.368599825388179</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -517,10 +517,10 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-3.094469838823551</v>
+        <v>3.094469838823552</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.376668031494518</v>
+        <v>-1.376668031494517</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -530,10 +530,10 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-3.085049872803416</v>
+        <v>3.085049872803417</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.533907049406036</v>
+        <v>-1.533907049406035</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -543,10 +543,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-3.19899807520926</v>
+        <v>3.198998075209261</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.819254367687724</v>
+        <v>-1.819254367687723</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -556,10 +556,10 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-3.49319377261856</v>
+        <v>3.493193772618561</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.361900046443284</v>
+        <v>-2.361900046443282</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -569,10 +569,10 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-4.107081945915393</v>
+        <v>4.107081945915395</v>
       </c>
       <c r="B11" t="n">
-        <v>-2.933374372939137</v>
+        <v>-2.933374372939135</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -582,10 +582,10 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-4.396406801887124</v>
+        <v>4.396406801887122</v>
       </c>
       <c r="B12" t="n">
-        <v>3.094855878672393</v>
+        <v>3.094855878672394</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -595,10 +595,10 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-8.296833649042719</v>
+        <v>8.296833649042719</v>
       </c>
       <c r="B13" t="n">
-        <v>2.476447878133517</v>
+        <v>2.47644787813352</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -608,10 +608,10 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-9.113499613078355</v>
+        <v>9.113499613078355</v>
       </c>
       <c r="B14" t="n">
-        <v>2.164240612167573</v>
+        <v>2.164240612167575</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -621,10 +621,10 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-7.706331351336996</v>
+        <v>7.706331351336996</v>
       </c>
       <c r="B15" t="n">
-        <v>0.1144095618874172</v>
+        <v>0.1144095618874198</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -634,10 +634,10 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-7.17716268125335</v>
+        <v>7.17716268125335</v>
       </c>
       <c r="B16" t="n">
-        <v>0.002021057133283306</v>
+        <v>0.002021057133285578</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -647,10 +647,10 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-6.889342251781858</v>
+        <v>6.889342251781858</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.2171235768468301</v>
+        <v>-0.2171235768468278</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -660,10 +660,10 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-6.971114139049122</v>
+        <v>6.971114139049123</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.09280447708341932</v>
+        <v>-0.0928044770834171</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -673,10 +673,10 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-4.655470022173076</v>
+        <v>4.655470022173077</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.1655708931914871</v>
+        <v>-0.1655708931914856</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>-4.43186321771539</v>
+        <v>4.43186321771539</v>
       </c>
       <c r="B20" t="n">
-        <v>1.126724835393274</v>
+        <v>1.126724835393275</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -699,7 +699,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>-4.25173119435592</v>
+        <v>4.251731194355919</v>
       </c>
       <c r="B21" t="n">
         <v>1.835110552620139</v>
@@ -712,7 +712,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.258904418307733</v>
+        <v>-1.258904418307731</v>
       </c>
       <c r="B22" t="n">
         <v>-3.437002747075447</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2.324363966962909</v>
+        <v>-2.324363966962907</v>
       </c>
       <c r="B23" t="n">
         <v>-3.97737543525612</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>3.33707219318659</v>
+        <v>-3.337072193186588</v>
       </c>
       <c r="B24" t="n">
         <v>-3.943234719665868</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3.935173222676871</v>
+        <v>-3.93517322267687</v>
       </c>
       <c r="B25" t="n">
         <v>-4.071290632159037</v>
@@ -764,10 +764,10 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>4.307895017720493</v>
+        <v>-4.307895017720491</v>
       </c>
       <c r="B26" t="n">
-        <v>-3.66066331995321</v>
+        <v>-3.660663319953211</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -777,10 +777,10 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>4.42868653474251</v>
+        <v>-4.428686534742507</v>
       </c>
       <c r="B27" t="n">
-        <v>-3.587544314311339</v>
+        <v>-3.58754431431134</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -790,10 +790,10 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>4.441669159107069</v>
+        <v>-4.441669159107067</v>
       </c>
       <c r="B28" t="n">
-        <v>-3.656649040980841</v>
+        <v>-3.656649040980843</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -803,10 +803,10 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>4.450981738091106</v>
+        <v>-4.450981738091104</v>
       </c>
       <c r="B29" t="n">
-        <v>-3.670067126249402</v>
+        <v>-3.670067126249404</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -816,10 +816,10 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>4.506151261384024</v>
+        <v>-4.506151261384021</v>
       </c>
       <c r="B30" t="n">
-        <v>-3.679986167529345</v>
+        <v>-3.679986167529346</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -829,10 +829,10 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>4.575497425582596</v>
+        <v>-4.575497425582594</v>
       </c>
       <c r="B31" t="n">
-        <v>-3.621203394294004</v>
+        <v>-3.621203394294005</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -842,10 +842,10 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1.790371385252494</v>
+        <v>-1.790371385252493</v>
       </c>
       <c r="B32" t="n">
-        <v>-2.221228988837776</v>
+        <v>-2.221228988837775</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -855,10 +855,10 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1.87456412876268</v>
+        <v>-1.874564128762678</v>
       </c>
       <c r="B33" t="n">
-        <v>-2.558503617819306</v>
+        <v>-2.558503617819305</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -868,10 +868,10 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1.249888594348886</v>
+        <v>-1.249888594348884</v>
       </c>
       <c r="B34" t="n">
-        <v>-2.75612413481044</v>
+        <v>-2.756124134810439</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -881,7 +881,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>-0.04813623307730648</v>
+        <v>0.04813623307730742</v>
       </c>
       <c r="B35" t="n">
         <v>-1.916932393284616</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>-0.003647797906353382</v>
+        <v>0.003647797906354298</v>
       </c>
       <c r="B36" t="n">
         <v>-1.923563491196187</v>
@@ -907,10 +907,10 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>-0.0296624899231731</v>
+        <v>0.02966248992317402</v>
       </c>
       <c r="B37" t="n">
-        <v>-1.918450176620017</v>
+        <v>-1.918450176620018</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -920,7 +920,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.07464520535350393</v>
+        <v>-0.07464520535350301</v>
       </c>
       <c r="B38" t="n">
         <v>-1.942109775529896</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.08101544037197578</v>
+        <v>-0.0810154403719749</v>
       </c>
       <c r="B39" t="n">
         <v>-1.854982729691148</v>
@@ -946,7 +946,7 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.04498100289363254</v>
+        <v>-0.04498100289363156</v>
       </c>
       <c r="B40" t="n">
         <v>-1.839901084364639</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>-0.1127559318595595</v>
+        <v>0.1127559318595604</v>
       </c>
       <c r="B41" t="n">
         <v>-1.744485440292353</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1.258611770072639</v>
+        <v>-1.258611770072641</v>
       </c>
       <c r="B42" t="n">
         <v>4.531728069684677</v>
@@ -985,10 +985,10 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1.137025233436898</v>
+        <v>-1.137025233436899</v>
       </c>
       <c r="B43" t="n">
-        <v>2.988321050428983</v>
+        <v>2.988321050428984</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -998,7 +998,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1.318083909845492</v>
+        <v>-1.318083909845494</v>
       </c>
       <c r="B44" t="n">
         <v>2.816273737860225</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1.335301828720229</v>
+        <v>-1.33530182872023</v>
       </c>
       <c r="B45" t="n">
         <v>2.482868935432966</v>
@@ -1024,10 +1024,10 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1.194214546023316</v>
+        <v>-1.194214546023317</v>
       </c>
       <c r="B46" t="n">
-        <v>2.227406223293864</v>
+        <v>2.227406223293865</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1037,10 +1037,10 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1.201579974256313</v>
+        <v>-1.201579974256314</v>
       </c>
       <c r="B47" t="n">
-        <v>2.040158387832352</v>
+        <v>2.040158387832353</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1.038129403412554</v>
+        <v>-1.038129403412555</v>
       </c>
       <c r="B48" t="n">
         <v>1.720726839523181</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.9524613910029454</v>
+        <v>-0.952461391002946</v>
       </c>
       <c r="B49" t="n">
         <v>1.462923813396934</v>
@@ -1076,10 +1076,10 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.9515072849613697</v>
+        <v>-0.9515072849613702</v>
       </c>
       <c r="B50" t="n">
-        <v>1.188274936281415</v>
+        <v>1.188274936281416</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2.14898117148814</v>
+        <v>-2.148981171488141</v>
       </c>
       <c r="B51" t="n">
         <v>1.111520777200537</v>
@@ -1102,10 +1102,10 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>4.589953370975738</v>
+        <v>-4.58995337097574</v>
       </c>
       <c r="B52" t="n">
-        <v>5.013217967960646</v>
+        <v>5.013217967960645</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1115,10 +1115,10 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>5.147183513040654</v>
+        <v>-5.147183513040655</v>
       </c>
       <c r="B53" t="n">
-        <v>2.834852379687788</v>
+        <v>2.834852379687787</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>4.48529166595462</v>
+        <v>-4.48529166595462</v>
       </c>
       <c r="B54" t="n">
         <v>2.003644101214671</v>
@@ -1141,10 +1141,10 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>5.442609514766506</v>
+        <v>-5.442609514766508</v>
       </c>
       <c r="B55" t="n">
-        <v>4.387207412801978</v>
+        <v>4.387207412801975</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>4.08619451622058</v>
+        <v>-4.086194516220583</v>
       </c>
       <c r="B56" t="n">
-        <v>4.268803532183066</v>
+        <v>4.268803532183063</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1167,10 +1167,10 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>4.324080457193888</v>
+        <v>-4.32408045719389</v>
       </c>
       <c r="B57" t="n">
-        <v>3.783399779369747</v>
+        <v>3.783399779369744</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1180,10 +1180,10 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>4.011154551280621</v>
+        <v>-4.011154551280622</v>
       </c>
       <c r="B58" t="n">
-        <v>3.302224127112818</v>
+        <v>3.302224127112816</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1193,10 +1193,10 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2.991809520133107</v>
+        <v>-2.991809520133108</v>
       </c>
       <c r="B59" t="n">
-        <v>2.801900124058112</v>
+        <v>2.801900124058109</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1206,10 +1206,10 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>3.402507780055235</v>
+        <v>-3.402507780055237</v>
       </c>
       <c r="B60" t="n">
-        <v>2.749048261755351</v>
+        <v>2.749048261755349</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1219,10 +1219,10 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>3.97369638710142</v>
+        <v>-3.973696387101422</v>
       </c>
       <c r="B61" t="n">
-        <v>4.663115561338598</v>
+        <v>4.663115561338596</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>

</xml_diff>